<commit_message>
Sample Excel 2007+ file (.xlsx)
</commit_message>
<xml_diff>
--- a/XL2ES_Example.xlsx
+++ b/XL2ES_Example.xlsx
@@ -417,7 +417,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -502,7 +504,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1">
         <v>31048</v>

</xml_diff>

<commit_message>
Incorporate the official Elasticsearch Perl client module
</commit_message>
<xml_diff>
--- a/XL2ES_Example.xlsx
+++ b/XL2ES_Example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="19980" windowHeight="8070"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Alan</t>
   </si>
@@ -73,6 +73,42 @@
   </si>
   <si>
     <t>Gagan</t>
+  </si>
+  <si>
+    <t>LastName_NS</t>
+  </si>
+  <si>
+    <t>Klark</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Khanna</t>
+  </si>
+  <si>
+    <t>Kapoor</t>
+  </si>
+  <si>
+    <t>Kunte</t>
+  </si>
+  <si>
+    <t>Address_AS</t>
+  </si>
+  <si>
+    <t>Bangalore India</t>
+  </si>
+  <si>
+    <t>Sydney Australia</t>
+  </si>
+  <si>
+    <t>PutraJaya Malaysia</t>
+  </si>
+  <si>
+    <t>Maharashtra India</t>
+  </si>
+  <si>
+    <t>Delhi India</t>
   </si>
 </sst>
 </file>
@@ -415,18 +451,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -434,79 +472,115 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2">
         <v>22</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="1">
         <v>29221</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3">
         <v>23</v>
       </c>
-      <c r="D3" s="1">
+      <c r="F3" s="1">
         <v>29952</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>102</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1">
         <v>30317</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>103</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5">
         <v>25</v>
       </c>
-      <c r="D5" s="1">
+      <c r="F5" s="1">
         <v>30682</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>104</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6">
         <v>28</v>
       </c>
-      <c r="D6" s="1">
+      <c r="F6" s="1">
         <v>31048</v>
       </c>
     </row>

</xml_diff>